<commit_message>
fix: Update Webasto ET Plants Excel file with all plants including 106
- Updated plant master data file to include all plants
- Ensures filter panel shows complete plant list on deployed version
- Fixes mismatch between localhost and Vercel deployment
</commit_message>
<xml_diff>
--- a/attachments/Webasto ET Plants .xlsx
+++ b/attachments/Webasto ET Plants .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://webasto-my.sharepoint.com/personal/george_neacsu_webasto_com/Documents/Desktop/QOS ET - Q Cockpit/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georg\QOS ET Report\attachments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{6256D46C-2E88-477F-AC8E-9894DDB66365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32AF892A-91F3-4DD9-98A8-6438B9043F11}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF96DAD2-E8A2-45E5-8E0E-1F3EFCCDD6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1283A2A6-0943-467A-8CD7-F606587A3C0C}"/>
+    <workbookView xWindow="28680" yWindow="2970" windowWidth="38640" windowHeight="15720" xr2:uid="{1283A2A6-0943-467A-8CD7-F606587A3C0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Webasto ET Plants" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
   <si>
     <t>City</t>
   </si>
@@ -287,7 +287,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1" xr:uid="{38C02465-EB1E-4F13-B02C-6EDC306ABAC9}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -304,7 +304,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -620,21 +620,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAEC9C27-1F7F-436B-97C6-826F16D56729}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D22"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="11" style="6"/>
-    <col min="3" max="3" width="18.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.09765625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -657,7 +657,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>101</v>
       </c>
@@ -680,457 +680,480 @@
         <v>13.260999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
+        <v>106</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3">
+        <v>17033</v>
+      </c>
+      <c r="F3" s="3">
+        <v>53.556899999999999</v>
+      </c>
+      <c r="G3" s="3">
+        <v>13.260999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>131</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="3">
-        <v>75100</v>
-      </c>
-      <c r="F3" s="3">
-        <v>44.55</v>
-      </c>
-      <c r="G3" s="3">
-        <v>26.065999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
-        <v>135</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="3">
-        <v>1138</v>
+        <v>75100</v>
       </c>
       <c r="F4" s="3">
-        <v>47.497900000000001</v>
+        <v>44.55</v>
       </c>
       <c r="G4" s="3">
-        <v>19.040199999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>26.065999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1138</v>
+      </c>
+      <c r="F5" s="3">
+        <v>47.497900000000001</v>
+      </c>
+      <c r="G5" s="3">
+        <v>19.040199999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>145</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F6" s="3">
         <v>53.522779999999997</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G6" s="3">
         <v>-1.1325000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+    <row r="7" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>155</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="3">
-        <v>44320</v>
-      </c>
-      <c r="F6" s="3">
-        <v>47.25</v>
-      </c>
-      <c r="G6" s="3">
-        <v>-2.0299999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
-        <v>111</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="3">
+        <v>44320</v>
+      </c>
+      <c r="F7" s="3">
+        <v>47.25</v>
+      </c>
+      <c r="G7" s="3">
+        <v>-2.0299999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>111</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
         <v>167</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E9" s="3">
         <v>40062</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F9" s="3">
         <v>44.615000000000002</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G9" s="3">
         <v>11.664999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
+    <row r="10" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
         <v>175</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="3">
-        <v>1230</v>
-      </c>
-      <c r="F9" s="3">
-        <v>48.208329999999997</v>
-      </c>
-      <c r="G9" s="3">
-        <v>16.372499999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
-        <v>180</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="E10" s="3">
-        <v>1000</v>
+        <v>1230</v>
       </c>
       <c r="F10" s="3">
-        <v>46.056899999999999</v>
+        <v>48.208329999999997</v>
       </c>
       <c r="G10" s="3">
-        <v>14.505800000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>16.372499999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>21</v>
+      <c r="E11" s="3">
+        <v>1000</v>
       </c>
       <c r="F11" s="3">
-        <v>48.716000000000001</v>
+        <v>46.056899999999999</v>
       </c>
       <c r="G11" s="3">
-        <v>21.260999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>14.505800000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F12" s="3">
-        <v>50.075499999999998</v>
+        <v>48.716000000000001</v>
       </c>
       <c r="G12" s="3">
-        <v>14.437799999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>21.260999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F13" s="3">
-        <v>52.334000000000003</v>
+        <v>50.075499999999998</v>
       </c>
       <c r="G13" s="3">
-        <v>20.885999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>14.437799999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="3">
+        <v>52.334000000000003</v>
+      </c>
+      <c r="G14" s="3">
+        <v>20.885999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>211</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="3">
-        <v>45030</v>
-      </c>
-      <c r="F14" s="3">
-        <v>38.619</v>
-      </c>
-      <c r="G14" s="3">
-        <v>27.428000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="5">
-        <v>215</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E15" s="3">
-        <v>34957</v>
+        <v>45030</v>
       </c>
       <c r="F15" s="3">
-        <v>40.816000000000003</v>
+        <v>38.619</v>
       </c>
       <c r="G15" s="3">
-        <v>29.3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>27.428000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="3">
+        <v>34957</v>
+      </c>
+      <c r="F16" s="3">
+        <v>40.816000000000003</v>
+      </c>
+      <c r="G16" s="3">
+        <v>29.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>230</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E17" s="3">
         <v>2610</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F17" s="3">
         <v>55.68</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G17" s="3">
         <v>12.452999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
+    <row r="18" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
         <v>235</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="3">
-        <v>8263</v>
-      </c>
-      <c r="F17" s="3">
-        <v>52.55</v>
-      </c>
-      <c r="G17" s="3">
-        <v>5.9169999999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
-        <v>410</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="E18" s="3">
-        <v>48430</v>
+        <v>8263</v>
       </c>
       <c r="F18" s="3">
-        <v>42.797780000000003</v>
+        <v>52.55</v>
       </c>
       <c r="G18" s="3">
-        <v>-83.704999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>5.9169999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="3">
+        <v>48430</v>
+      </c>
+      <c r="F19" s="3">
+        <v>42.797780000000003</v>
+      </c>
+      <c r="G19" s="3">
+        <v>-83.704999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>411</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F20" s="3">
         <v>34.148000000000003</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G20" s="3">
         <v>-118</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="5">
+    <row r="21" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
         <v>705</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="3">
-        <v>35.4437</v>
-      </c>
-      <c r="G20" s="3">
-        <v>139.63800000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="5">
-        <v>752</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>54</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="3">
-        <v>430056</v>
+        <v>45</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="F21" s="3">
-        <v>30.5928</v>
+        <v>35.4437</v>
       </c>
       <c r="G21" s="3">
-        <v>114.30549999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+        <v>139.63800000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>770</v>
+        <v>752</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>54</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>46</v>
       </c>
       <c r="E22" s="3">
+        <v>430056</v>
+      </c>
+      <c r="F22" s="3">
+        <v>30.5928</v>
+      </c>
+      <c r="G22" s="3">
+        <v>114.30549999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>770</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="3">
         <v>100105</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F23" s="3">
         <v>39.904200000000003</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G23" s="3">
         <v>116.4074</v>
       </c>
     </row>

</xml_diff>